<commit_message>
actualizacion 13 de junio
-Graficas por dia, mes, año y total de los paneles solares.
-Creacion de menu personalizado para el administrador
-Modificacion de las vistas de inventario y sistemas fotovoltaicos del administrador
</commit_message>
<xml_diff>
--- a/crontabs/investormeasures/archivo CVS.xlsx
+++ b/crontabs/investormeasures/archivo CVS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\Dropbox\GS_Ejecutivo_Shared\C05-CIDETEC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\finbaproject\FINBA\crontabs\investormeasures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,31 +21,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Fecha y hora,Energía por inversor|FRONIUS Symo 15.0-3 208 (1) (# 1),Energía por inversor por kWp|FRONIUS Symo 15.0-3 208 (1) (# 1),Instalación total,</t>
-  </si>
-  <si>
     <t>[dd.MM.yyyy],[kWh],[kWh/kWp],[kWh],</t>
   </si>
   <si>
-    <t>08.05.2019,81.76,5.41,81.76,</t>
+    <t>01.01.2019,81.76,5.41,81.76,</t>
   </si>
   <si>
-    <t>09.05.2019,70.85,4.69,70.85,</t>
+    <t>07.01.2019,70.85,4.69,70.85,</t>
   </si>
   <si>
-    <t>10.05.2019,81.23,5.37,81.23,</t>
+    <t>09.01.2019,81.23,5.37,81.23,</t>
   </si>
   <si>
-    <t>11.05.2019,76.61,5.07,76.61,</t>
+    <t>14.01.2019,76.61,5.07,76.61,</t>
   </si>
   <si>
-    <t>12.05.2019,62.62,4.14,62.62,</t>
+    <t>16.01.2019,62.62,4.14,62.62,</t>
   </si>
   <si>
-    <t>13.05.2019,63.90,4.23,63.90,</t>
+    <t>21.01.2019,63.90,4.23,63.90,</t>
   </si>
   <si>
-    <t>14.05.2019,21.67,1.43,21.67,</t>
+    <t>30.01.2019,21.67,1.43,21.67,</t>
+  </si>
+  <si>
+    <t>Fecha y hora,Energía por inversor|FRONIUS Symo 22.7-3 kW 1,Energía por inversor por kWp|FRONIUS Symo 22.7-3 kW 1,Instalación total,</t>
   </si>
 </sst>
 </file>
@@ -576,8 +576,36 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -860,50 +888,51 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>